<commit_message>
Add XLSX parser for mining pools; electricity calculations
</commit_message>
<xml_diff>
--- a/data/Pool_data_final.xlsx
+++ b/data/Pool_data_final.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="May 17 2021" sheetId="1" state="visible" r:id="rId2"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1820" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1820" uniqueCount="109">
   <si>
     <t xml:space="preserve">Pools</t>
   </si>
@@ -134,7 +134,7 @@
     <t xml:space="preserve">0.09674</t>
   </si>
   <si>
-    <t xml:space="preserve">New Jersey, United States</t>
+    <t xml:space="preserve">North Bergen, New Jersey, United States</t>
   </si>
   <si>
     <t xml:space="preserve">0.2233</t>
@@ -275,9 +275,6 @@
     <t xml:space="preserve">0.55304</t>
   </si>
   <si>
-    <t xml:space="preserve">North Bergen, New Jersey, United States</t>
-  </si>
-  <si>
     <t xml:space="preserve">SBI Crypto</t>
   </si>
   <si>
@@ -296,34 +293,13 @@
     <t xml:space="preserve">United States of America,Washington,Seattle</t>
   </si>
   <si>
-    <t xml:space="preserve">Netherlands,Noord-Holland,Amsterdam</t>
-  </si>
-  <si>
     <t xml:space="preserve">United States of America,New Jersey,Clifton</t>
   </si>
   <si>
     <t xml:space="preserve">United States of America, New Jersey, North Bergen</t>
   </si>
   <si>
-    <t xml:space="preserve">United States of America,Virginia,Ashburn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">United States of America,New Jersey,North Bergen</t>
-  </si>
-  <si>
     <t xml:space="preserve">Brazil,Sao Paulo,Sao Paulo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Canada,Quebec,Montreal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Canada,Ontario,Toronto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Japan,Tokyo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Russian Federation,Moskva,Moscow</t>
   </si>
   <si>
     <t xml:space="preserve">Kazakhstan,Almaty</t>
@@ -353,9 +329,6 @@
     <t xml:space="preserve">EMCDPool</t>
   </si>
   <si>
-    <t xml:space="preserve">Russian Federation,Sankt-Peterburg,Saint Petersburg</t>
-  </si>
-  <si>
     <t xml:space="preserve">Germany,Sachsen,Falkenstein</t>
   </si>
   <si>
@@ -368,19 +341,10 @@
     <t xml:space="preserve">Kazakhstan,Qaraghandy oblysy,Kazakhstan</t>
   </si>
   <si>
-    <t xml:space="preserve">China,Beijing</t>
-  </si>
-  <si>
     <t xml:space="preserve">China,Sichuan,Chengdu</t>
   </si>
   <si>
     <t xml:space="preserve">United States of America,Illinoise,Chicago</t>
-  </si>
-  <si>
-    <t xml:space="preserve">United States of America, Colorado, Greenwood Village</t>
-  </si>
-  <si>
-    <t xml:space="preserve">United States of America,Texas,Dallas</t>
   </si>
   <si>
     <t xml:space="preserve">United States of America,District of Columbia,Washington</t>
@@ -389,10 +353,7 @@
     <t xml:space="preserve">United States of America,California,San Francisco</t>
   </si>
   <si>
-    <t xml:space="preserve">China,Beijing,Beijing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">United States of America,New York,New York City</t>
+    <t xml:space="preserve">Beijing, China,Beijing</t>
   </si>
   <si>
     <t xml:space="preserve">United States of America,California,Sacramento</t>
@@ -402,6 +363,9 @@
   </si>
   <si>
     <t xml:space="preserve">United Kingdom,England,London</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eu</t>
   </si>
   <si>
     <t xml:space="preserve">United States of America,Utah,Provo</t>
@@ -933,11 +897,11 @@
   </sheetPr>
   <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A23" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C43" activeCellId="0" sqref="C43"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F41" activeCellId="0" sqref="F41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.53125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.33"/>
@@ -2881,11 +2845,11 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A33" activeCellId="0" sqref="A33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.53125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.83"/>
@@ -3341,7 +3305,7 @@
         <v>39</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>76</v>
+        <v>29</v>
       </c>
       <c r="C23" s="9" t="n">
         <v>0.2233</v>
@@ -3458,7 +3422,7 @@
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>7</v>
@@ -3478,7 +3442,7 @@
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>19</v>
@@ -3498,7 +3462,7 @@
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>48</v>
@@ -4525,11 +4489,11 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.53125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.83"/>
@@ -4864,7 +4828,7 @@
         <v>39</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>76</v>
+        <v>29</v>
       </c>
       <c r="C17" s="9" t="n">
         <v>0.2233</v>
@@ -4981,7 +4945,7 @@
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>7</v>
@@ -5001,7 +4965,7 @@
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>19</v>
@@ -5021,7 +4985,7 @@
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>48</v>
@@ -6032,14 +5996,14 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A105" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A119" activeCellId="0" sqref="A119"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A33" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H80" activeCellId="0" sqref="H80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.53125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="75.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="8" width="34.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.67"/>
@@ -6051,7 +6015,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -6074,19 +6038,19 @@
         <v>6</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C2" s="9" t="n">
         <v>0.514658864</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6094,19 +6058,19 @@
         <v>18</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C3" s="9" t="n">
         <v>0.514658864</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6114,19 +6078,19 @@
         <v>18</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C4" s="9" t="n">
         <v>0.514658864</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6134,19 +6098,19 @@
         <v>18</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C5" s="9" t="n">
         <v>0.514658864</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6154,19 +6118,19 @@
         <v>17</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C6" s="9" t="n">
         <v>0.514658864</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6174,7 +6138,7 @@
         <v>17</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C7" s="22" t="n">
         <v>0.58883</v>
@@ -6194,19 +6158,19 @@
         <v>17</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C8" s="9" t="n">
         <v>0.514658864</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6214,19 +6178,19 @@
         <v>31</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C9" s="9" t="n">
         <v>0.514658864</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6234,19 +6198,19 @@
         <v>31</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C10" s="9" t="n">
         <v>0.514658864</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6274,7 +6238,7 @@
         <v>31</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C12" s="24" t="n">
         <v>0.09674</v>
@@ -6294,7 +6258,7 @@
         <v>31</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C13" s="22" t="n">
         <v>0.09674</v>
@@ -6314,19 +6278,19 @@
         <v>25</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C14" s="9" t="n">
         <v>0.514658864</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6334,19 +6298,19 @@
         <v>25</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C15" s="9" t="n">
         <v>0.514658864</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6354,7 +6318,7 @@
         <v>39</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>83</v>
+        <v>42</v>
       </c>
       <c r="C16" s="22" t="n">
         <v>0.45172</v>
@@ -6374,7 +6338,7 @@
         <v>39</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C17" s="24" t="n">
         <v>0.58883</v>
@@ -6394,7 +6358,7 @@
         <v>39</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C18" s="22" t="n">
         <v>0.2233</v>
@@ -6414,7 +6378,7 @@
         <v>39</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C19" s="24" t="n">
         <v>0.2233</v>
@@ -6434,7 +6398,7 @@
         <v>39</v>
       </c>
       <c r="B20" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C20" s="22" t="n">
         <v>0.58883</v>
@@ -6454,7 +6418,7 @@
         <v>39</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C21" s="24" t="n">
         <v>0.2233</v>
@@ -6474,7 +6438,7 @@
         <v>39</v>
       </c>
       <c r="B22" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C22" s="22" t="n">
         <v>0.58883</v>
@@ -6494,7 +6458,7 @@
         <v>39</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>83</v>
+        <v>42</v>
       </c>
       <c r="C23" s="24" t="n">
         <v>0.45172</v>
@@ -6514,7 +6478,7 @@
         <v>39</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C24" s="22" t="n">
         <v>0.58883</v>
@@ -6534,7 +6498,7 @@
         <v>39</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>86</v>
+        <v>10</v>
       </c>
       <c r="C25" s="24" t="n">
         <v>0.2925</v>
@@ -6554,7 +6518,7 @@
         <v>39</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C26" s="22" t="n">
         <v>0.58883</v>
@@ -6574,7 +6538,7 @@
         <v>39</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>86</v>
+        <v>10</v>
       </c>
       <c r="C27" s="24" t="n">
         <v>0.2925</v>
@@ -6594,7 +6558,7 @@
         <v>39</v>
       </c>
       <c r="B28" s="21" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C28" s="22" t="n">
         <v>0.2233</v>
@@ -6614,7 +6578,7 @@
         <v>39</v>
       </c>
       <c r="B29" s="23" t="s">
-        <v>86</v>
+        <v>10</v>
       </c>
       <c r="C29" s="24" t="n">
         <v>0.2925</v>
@@ -6634,7 +6598,7 @@
         <v>39</v>
       </c>
       <c r="B30" s="21" t="s">
-        <v>86</v>
+        <v>10</v>
       </c>
       <c r="C30" s="22" t="n">
         <v>0.2925</v>
@@ -6654,7 +6618,7 @@
         <v>39</v>
       </c>
       <c r="B31" s="23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C31" s="24" t="n">
         <v>0.58883</v>
@@ -6674,7 +6638,7 @@
         <v>39</v>
       </c>
       <c r="B32" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C32" s="22" t="n">
         <v>0.58883</v>
@@ -6694,7 +6658,7 @@
         <v>39</v>
       </c>
       <c r="B33" s="23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C33" s="24" t="n">
         <v>0.58883</v>
@@ -6714,7 +6678,7 @@
         <v>39</v>
       </c>
       <c r="B34" s="21" t="s">
-        <v>83</v>
+        <v>42</v>
       </c>
       <c r="C34" s="22" t="n">
         <v>0.45172</v>
@@ -6734,7 +6698,7 @@
         <v>39</v>
       </c>
       <c r="B35" s="23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C35" s="24" t="n">
         <v>0.58883</v>
@@ -6754,7 +6718,7 @@
         <v>39</v>
       </c>
       <c r="B36" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C36" s="22" t="n">
         <v>0.58883</v>
@@ -6774,7 +6738,7 @@
         <v>39</v>
       </c>
       <c r="B37" s="23" t="s">
-        <v>83</v>
+        <v>42</v>
       </c>
       <c r="C37" s="24" t="n">
         <v>0.45172</v>
@@ -6794,7 +6758,7 @@
         <v>39</v>
       </c>
       <c r="B38" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C38" s="22" t="n">
         <v>0.58883</v>
@@ -6814,7 +6778,7 @@
         <v>39</v>
       </c>
       <c r="B39" s="23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C39" s="24" t="n">
         <v>0.58883</v>
@@ -6834,7 +6798,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C40" s="22" t="n">
         <v>0.2233</v>
@@ -6854,7 +6818,7 @@
         <v>39</v>
       </c>
       <c r="B41" s="23" t="s">
-        <v>86</v>
+        <v>10</v>
       </c>
       <c r="C41" s="24" t="n">
         <v>0.2925</v>
@@ -6874,7 +6838,7 @@
         <v>39</v>
       </c>
       <c r="B42" s="21" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C42" s="22" t="n">
         <v>0.2233</v>
@@ -6894,7 +6858,7 @@
         <v>39</v>
       </c>
       <c r="B43" s="23" t="s">
-        <v>86</v>
+        <v>10</v>
       </c>
       <c r="C43" s="24" t="n">
         <v>0.2925</v>
@@ -6914,7 +6878,7 @@
         <v>39</v>
       </c>
       <c r="B44" s="21" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C44" s="22" t="n">
         <v>0.2233</v>
@@ -6934,7 +6898,7 @@
         <v>39</v>
       </c>
       <c r="B45" s="23" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C45" s="24" t="n">
         <v>0.2233</v>
@@ -6954,7 +6918,7 @@
         <v>39</v>
       </c>
       <c r="B46" s="21" t="s">
-        <v>86</v>
+        <v>10</v>
       </c>
       <c r="C46" s="22" t="n">
         <v>0.2925</v>
@@ -6974,7 +6938,7 @@
         <v>39</v>
       </c>
       <c r="B47" s="23" t="s">
-        <v>86</v>
+        <v>10</v>
       </c>
       <c r="C47" s="24" t="n">
         <v>0.2925</v>
@@ -6994,7 +6958,7 @@
         <v>39</v>
       </c>
       <c r="B48" s="21" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C48" s="22" t="n">
         <v>0.0617</v>
@@ -7014,7 +6978,7 @@
         <v>39</v>
       </c>
       <c r="B49" s="23" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="C49" s="24" t="n">
         <v>0.0012</v>
@@ -7034,7 +6998,7 @@
         <v>39</v>
       </c>
       <c r="B50" s="21" t="s">
-        <v>90</v>
+        <v>44</v>
       </c>
       <c r="C50" s="22" t="n">
         <v>0.03</v>
@@ -7054,7 +7018,7 @@
         <v>39</v>
       </c>
       <c r="B51" s="23" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="C51" s="24" t="n">
         <v>0.0012</v>
@@ -7074,7 +7038,7 @@
         <v>39</v>
       </c>
       <c r="B52" s="21" t="s">
-        <v>90</v>
+        <v>44</v>
       </c>
       <c r="C52" s="22" t="n">
         <v>0.03</v>
@@ -7094,7 +7058,7 @@
         <v>39</v>
       </c>
       <c r="B53" s="23" t="s">
-        <v>90</v>
+        <v>44</v>
       </c>
       <c r="C53" s="24" t="n">
         <v>0.03</v>
@@ -7114,7 +7078,7 @@
         <v>39</v>
       </c>
       <c r="B54" s="21" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="C54" s="22" t="n">
         <v>0.0012</v>
@@ -7134,7 +7098,7 @@
         <v>39</v>
       </c>
       <c r="B55" s="23" t="s">
-        <v>90</v>
+        <v>44</v>
       </c>
       <c r="C55" s="24" t="n">
         <v>0.03</v>
@@ -7154,7 +7118,7 @@
         <v>39</v>
       </c>
       <c r="B56" s="21" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="C56" s="22" t="n">
         <v>0.0012</v>
@@ -7214,7 +7178,7 @@
         <v>39</v>
       </c>
       <c r="B59" s="23" t="s">
-        <v>91</v>
+        <v>48</v>
       </c>
       <c r="C59" s="24" t="n">
         <v>0.4658</v>
@@ -7234,7 +7198,7 @@
         <v>39</v>
       </c>
       <c r="B60" s="21" t="s">
-        <v>91</v>
+        <v>48</v>
       </c>
       <c r="C60" s="22" t="n">
         <v>0.4658</v>
@@ -7254,7 +7218,7 @@
         <v>39</v>
       </c>
       <c r="B61" s="23" t="s">
-        <v>92</v>
+        <v>50</v>
       </c>
       <c r="C61" s="24" t="n">
         <v>0.3102</v>
@@ -7274,7 +7238,7 @@
         <v>39</v>
       </c>
       <c r="B62" s="21" t="s">
-        <v>92</v>
+        <v>50</v>
       </c>
       <c r="C62" s="22" t="n">
         <v>0.3102</v>
@@ -7294,13 +7258,13 @@
         <v>39</v>
       </c>
       <c r="B63" s="23" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C63" s="24" t="n">
         <v>0.516</v>
       </c>
       <c r="D63" s="23" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="E63" s="6" t="n">
         <v>43.25</v>
@@ -7311,10 +7275,10 @@
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="18" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="B64" s="21" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="C64" s="22" t="n">
         <v>0.7341</v>
@@ -7334,7 +7298,7 @@
         <v>26</v>
       </c>
       <c r="B65" s="23" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="C65" s="9" t="n">
         <v>0.377155625</v>
@@ -7354,7 +7318,7 @@
         <v>26</v>
       </c>
       <c r="B66" s="21" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="C66" s="22" t="n">
         <v>0.42394</v>
@@ -7394,7 +7358,7 @@
         <v>70</v>
       </c>
       <c r="B68" s="21" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C68" s="22" t="n">
         <v>0.56848</v>
@@ -7414,7 +7378,7 @@
         <v>70</v>
       </c>
       <c r="B69" s="23" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C69" s="24" t="n">
         <v>0.56848</v>
@@ -7434,7 +7398,7 @@
         <v>70</v>
       </c>
       <c r="B70" s="21" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C70" s="22" t="n">
         <v>0.56848</v>
@@ -7451,10 +7415,10 @@
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B71" s="23" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="C71" s="24" t="n">
         <v>0.15495</v>
@@ -7471,10 +7435,10 @@
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B72" s="21" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="C72" s="22" t="n">
         <v>0.15495</v>
@@ -7491,10 +7455,10 @@
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B73" s="23" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="C73" s="24" t="n">
         <v>0.15495</v>
@@ -7511,10 +7475,10 @@
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B74" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C74" s="22" t="n">
         <v>0.58883</v>
@@ -7531,10 +7495,10 @@
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B75" s="23" t="s">
-        <v>91</v>
+        <v>48</v>
       </c>
       <c r="C75" s="24" t="n">
         <v>0.4658</v>
@@ -7551,10 +7515,10 @@
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="18" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B76" s="21" t="s">
-        <v>102</v>
+        <v>59</v>
       </c>
       <c r="C76" s="22" t="n">
         <v>0.3102</v>
@@ -7571,10 +7535,10 @@
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="18" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B77" s="23" t="s">
-        <v>102</v>
+        <v>59</v>
       </c>
       <c r="C77" s="24" t="n">
         <v>0.3102</v>
@@ -7591,10 +7555,10 @@
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="18" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B78" s="21" t="s">
-        <v>102</v>
+        <v>59</v>
       </c>
       <c r="C78" s="22" t="n">
         <v>0.3102</v>
@@ -7611,10 +7575,10 @@
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="18" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B79" s="23" t="s">
-        <v>102</v>
+        <v>59</v>
       </c>
       <c r="C79" s="24" t="n">
         <v>0.3102</v>
@@ -7631,10 +7595,10 @@
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="18" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B80" s="21" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="C80" s="22" t="n">
         <v>0.58883</v>
@@ -7651,10 +7615,10 @@
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="18" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B81" s="23" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="C81" s="24" t="n">
         <v>0.26818</v>
@@ -7671,7 +7635,7 @@
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="18" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B82" s="21" t="s">
         <v>53</v>
@@ -7691,10 +7655,10 @@
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="18" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B83" s="23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C83" s="24" t="n">
         <v>0.09674</v>
@@ -7711,10 +7675,10 @@
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="18" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B84" s="21" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="C84" s="22" t="n">
         <v>0.700153846</v>
@@ -7731,16 +7695,16 @@
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="18" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B85" s="23" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="C85" s="24" t="n">
         <v>0.516</v>
       </c>
       <c r="D85" s="23" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="E85" s="6" t="n">
         <v>48.51667</v>
@@ -7794,7 +7758,7 @@
         <v>35</v>
       </c>
       <c r="B88" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C88" s="22" t="n">
         <v>0.58883</v>
@@ -7814,7 +7778,7 @@
         <v>35</v>
       </c>
       <c r="B89" s="23" t="s">
-        <v>107</v>
+        <v>37</v>
       </c>
       <c r="C89" s="24" t="n">
         <v>0.982118481</v>
@@ -7834,7 +7798,7 @@
         <v>35</v>
       </c>
       <c r="B90" s="21" t="s">
-        <v>107</v>
+        <v>37</v>
       </c>
       <c r="C90" s="22" t="n">
         <v>0.982118481</v>
@@ -7854,7 +7818,7 @@
         <v>35</v>
       </c>
       <c r="B91" s="23" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="C91" s="24" t="n">
         <v>0.982118481</v>
@@ -7874,7 +7838,7 @@
         <v>58</v>
       </c>
       <c r="B92" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C92" s="22" t="n">
         <v>0.58883</v>
@@ -7894,7 +7858,7 @@
         <v>58</v>
       </c>
       <c r="B93" s="23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C93" s="24" t="n">
         <v>0.58883</v>
@@ -7914,7 +7878,7 @@
         <v>58</v>
       </c>
       <c r="B94" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C94" s="22" t="n">
         <v>0.58883</v>
@@ -7934,7 +7898,7 @@
         <v>58</v>
       </c>
       <c r="B95" s="23" t="s">
-        <v>102</v>
+        <v>59</v>
       </c>
       <c r="C95" s="24" t="n">
         <v>0.3102</v>
@@ -7954,7 +7918,7 @@
         <v>58</v>
       </c>
       <c r="B96" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C96" s="22" t="n">
         <v>0.58883</v>
@@ -7974,7 +7938,7 @@
         <v>58</v>
       </c>
       <c r="B97" s="23" t="s">
-        <v>102</v>
+        <v>59</v>
       </c>
       <c r="C97" s="24" t="n">
         <v>0.3102</v>
@@ -7994,7 +7958,7 @@
         <v>58</v>
       </c>
       <c r="B98" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C98" s="22" t="n">
         <v>0.58883</v>
@@ -8014,7 +7978,7 @@
         <v>58</v>
       </c>
       <c r="B99" s="23" t="s">
-        <v>102</v>
+        <v>59</v>
       </c>
       <c r="C99" s="24" t="n">
         <v>0.3102</v>
@@ -8034,7 +7998,7 @@
         <v>58</v>
       </c>
       <c r="B100" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C100" s="22" t="n">
         <v>0.58883</v>
@@ -8054,7 +8018,7 @@
         <v>33</v>
       </c>
       <c r="B101" s="23" t="s">
-        <v>107</v>
+        <v>37</v>
       </c>
       <c r="C101" s="24" t="n">
         <v>0.982118481</v>
@@ -8074,7 +8038,7 @@
         <v>33</v>
       </c>
       <c r="B102" s="21" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="C102" s="22" t="n">
         <v>0.2524</v>
@@ -8094,7 +8058,7 @@
         <v>33</v>
       </c>
       <c r="B103" s="23" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
       <c r="C103" s="24" t="n">
         <v>0.38896</v>
@@ -8114,7 +8078,7 @@
         <v>33</v>
       </c>
       <c r="B104" s="21" t="s">
-        <v>111</v>
+        <v>67</v>
       </c>
       <c r="C104" s="22" t="n">
         <v>0.38896</v>
@@ -8134,7 +8098,7 @@
         <v>33</v>
       </c>
       <c r="B105" s="23" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="C105" s="24" t="n">
         <v>0.36338</v>
@@ -8154,7 +8118,7 @@
         <v>33</v>
       </c>
       <c r="B106" s="21" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="C106" s="22" t="n">
         <v>0.20553</v>
@@ -8174,7 +8138,7 @@
         <v>33</v>
       </c>
       <c r="B107" s="23" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="C107" s="24" t="n">
         <v>0.2524</v>
@@ -8194,7 +8158,7 @@
         <v>33</v>
       </c>
       <c r="B108" s="21" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="C108" s="22" t="n">
         <v>0.20553</v>
@@ -8214,7 +8178,7 @@
         <v>33</v>
       </c>
       <c r="B109" s="23" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="C109" s="24" t="n">
         <v>0.982118481</v>
@@ -8234,7 +8198,7 @@
         <v>33</v>
       </c>
       <c r="B110" s="21" t="s">
-        <v>115</v>
+        <v>40</v>
       </c>
       <c r="C110" s="22" t="n">
         <v>0.18901</v>
@@ -8254,7 +8218,7 @@
         <v>33</v>
       </c>
       <c r="B111" s="23" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="C111" s="24" t="n">
         <v>0.20553</v>
@@ -8274,7 +8238,7 @@
         <v>33</v>
       </c>
       <c r="B112" s="21" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="C112" s="22" t="n">
         <v>0.20553</v>
@@ -8294,7 +8258,7 @@
         <v>33</v>
       </c>
       <c r="B113" s="23" t="s">
-        <v>111</v>
+        <v>67</v>
       </c>
       <c r="C113" s="24" t="n">
         <v>0.38896</v>
@@ -8314,7 +8278,7 @@
         <v>33</v>
       </c>
       <c r="B114" s="21" t="s">
-        <v>107</v>
+        <v>37</v>
       </c>
       <c r="C114" s="22" t="n">
         <v>0.982118481</v>
@@ -8334,7 +8298,7 @@
         <v>33</v>
       </c>
       <c r="B115" s="23" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="C115" s="24" t="n">
         <v>0.20553</v>
@@ -8354,7 +8318,7 @@
         <v>33</v>
       </c>
       <c r="B116" s="21" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="C116" s="22" t="n">
         <v>0.01152</v>
@@ -8394,7 +8358,7 @@
         <v>33</v>
       </c>
       <c r="B118" s="21" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="C118" s="22" t="n">
         <v>0.21233</v>
@@ -8411,10 +8375,10 @@
     </row>
     <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A119" s="27" t="s">
-        <v>33</v>
+        <v>106</v>
       </c>
       <c r="B119" s="23" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="C119" s="24" t="n">
         <v>0.20553</v>
@@ -8434,7 +8398,7 @@
         <v>33</v>
       </c>
       <c r="B120" s="21" t="s">
-        <v>111</v>
+        <v>67</v>
       </c>
       <c r="C120" s="22" t="n">
         <v>0.38896</v>
@@ -8454,7 +8418,7 @@
         <v>33</v>
       </c>
       <c r="B121" s="23" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="C121" s="24" t="n">
         <v>0.71022</v>
@@ -8494,7 +8458,7 @@
         <v>33</v>
       </c>
       <c r="B123" s="23" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="C123" s="24" t="n">
         <v>0.71022</v>
@@ -8514,7 +8478,7 @@
         <v>56</v>
       </c>
       <c r="B124" s="21" t="s">
-        <v>107</v>
+        <v>37</v>
       </c>
       <c r="C124" s="22" t="n">
         <v>0.982118481</v>
@@ -9437,11 +9401,11 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A20" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E53" activeCellId="0" sqref="E53"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C14" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.53125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.5"/>
@@ -11384,11 +11348,11 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A49" activeCellId="0" sqref="A49"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.53125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.5"/>
@@ -13332,8 +13296,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A21" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A48" activeCellId="0" sqref="A48"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C30" activeCellId="0" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15262,11 +15226,11 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A33" activeCellId="0" sqref="A33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.53125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.83"/>
@@ -15722,7 +15686,7 @@
         <v>39</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>76</v>
+        <v>29</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>30</v>
@@ -15839,7 +15803,7 @@
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>7</v>
@@ -15859,7 +15823,7 @@
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>19</v>
@@ -15879,7 +15843,7 @@
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>48</v>
@@ -16906,11 +16870,11 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A33" activeCellId="0" sqref="A33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.53125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.83"/>
@@ -17362,7 +17326,7 @@
         <v>39</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>76</v>
+        <v>29</v>
       </c>
       <c r="C23" s="9" t="n">
         <v>0.2233</v>
@@ -17479,7 +17443,7 @@
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>7</v>
@@ -17499,7 +17463,7 @@
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>19</v>
@@ -17519,7 +17483,7 @@
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>48</v>
@@ -18546,11 +18510,11 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A33" activeCellId="0" sqref="A33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.53125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.83"/>
@@ -19006,7 +18970,7 @@
         <v>39</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>76</v>
+        <v>29</v>
       </c>
       <c r="C23" s="9" t="n">
         <v>0.2233</v>
@@ -19123,7 +19087,7 @@
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>7</v>
@@ -19143,7 +19107,7 @@
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>19</v>
@@ -19163,7 +19127,7 @@
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>48</v>
@@ -20190,11 +20154,11 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A33" activeCellId="0" sqref="A33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E52" activeCellId="0" sqref="E52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.53125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.83"/>
@@ -20650,7 +20614,7 @@
         <v>39</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>76</v>
+        <v>29</v>
       </c>
       <c r="C23" s="9" t="n">
         <v>0.2233</v>
@@ -20767,7 +20731,7 @@
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>7</v>
@@ -20787,7 +20751,7 @@
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>19</v>
@@ -20807,7 +20771,7 @@
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>48</v>
@@ -21834,11 +21798,11 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A33" activeCellId="0" sqref="A33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.53125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.83"/>
@@ -22294,7 +22258,7 @@
         <v>39</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>76</v>
+        <v>29</v>
       </c>
       <c r="C23" s="9" t="n">
         <v>0.2233</v>
@@ -22411,7 +22375,7 @@
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>7</v>
@@ -22431,7 +22395,7 @@
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>19</v>
@@ -22451,7 +22415,7 @@
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>48</v>

</xml_diff>

<commit_message>
Deploy-ready version; CO2 API Alpha v0.1
</commit_message>
<xml_diff>
--- a/data/Pool_data_final.xlsx
+++ b/data/Pool_data_final.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Jan 01 2021" sheetId="1" state="visible" r:id="rId2"/>
@@ -793,7 +793,7 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A49" activeCellId="0" sqref="A49"/>
     </sheetView>
   </sheetViews>
@@ -10768,8 +10768,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A125" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A125" activeCellId="0" sqref="A125"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B36" activeCellId="0" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Add del command & fix split between unknown sources
</commit_message>
<xml_diff>
--- a/data/Pool_data_final.xlsx
+++ b/data/Pool_data_final.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Jan 01 2021" sheetId="1" state="visible" r:id="rId2"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1525" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1543" uniqueCount="105">
   <si>
     <t xml:space="preserve">Pools</t>
   </si>
@@ -227,6 +227,9 @@
     <t xml:space="preserve">OurWorldInData</t>
   </si>
   <si>
+    <t xml:space="preserve">Pools with no server info</t>
+  </si>
+  <si>
     <t xml:space="preserve">Latitude </t>
   </si>
   <si>
@@ -355,7 +358,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -400,18 +403,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="4">
@@ -508,7 +499,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="31">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -617,20 +608,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -638,14 +621,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -793,11 +768,11 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A49" activeCellId="0" sqref="A49"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A60" activeCellId="0" sqref="A60:F60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.33"/>
@@ -1988,7 +1963,26 @@
         <v>-38.193144</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B60" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C60" s="8" t="n">
+        <v>0.442</v>
+      </c>
+      <c r="D60" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="E60" s="4" t="n">
+        <v>40.527483</v>
+      </c>
+      <c r="F60" s="5" t="n">
+        <v>-38.193144</v>
+      </c>
+    </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2948,10 +2942,10 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A20" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A49" activeCellId="0" sqref="A49"/>
+      <selection pane="topLeft" activeCell="A60" activeCellId="0" sqref="A60:F60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.33"/>
@@ -4142,7 +4136,26 @@
         <v>-38.193144</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B60" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C60" s="8" t="n">
+        <v>0.442</v>
+      </c>
+      <c r="D60" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="E60" s="4" t="n">
+        <v>40.527483</v>
+      </c>
+      <c r="F60" s="5" t="n">
+        <v>-38.193144</v>
+      </c>
+    </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -5102,7 +5115,7 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A24" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A48" activeCellId="0" sqref="A48"/>
+      <selection pane="topLeft" activeCell="A59" activeCellId="1" sqref="A60:F60 A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5131,10 +5144,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6277,7 +6290,26 @@
         <v>-38.193144</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B59" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C59" s="8" t="n">
+        <v>0.442</v>
+      </c>
+      <c r="D59" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="E59" s="4" t="n">
+        <v>40.527483</v>
+      </c>
+      <c r="F59" s="5" t="n">
+        <v>-38.193144</v>
+      </c>
+    </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -7241,10 +7273,10 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A33" activeCellId="0" sqref="A33"/>
+      <selection pane="topLeft" activeCell="A43" activeCellId="1" sqref="A60:F60 A43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.83"/>
@@ -7269,10 +7301,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7280,7 +7312,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>13</v>
@@ -7300,10 +7332,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>9</v>
@@ -7343,7 +7375,7 @@
         <v>46</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>9</v>
@@ -7360,7 +7392,7 @@
         <v>18</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>13</v>
@@ -7380,10 +7412,10 @@
         <v>18</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>9</v>
@@ -7420,7 +7452,7 @@
         <v>25</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>13</v>
@@ -7520,7 +7552,7 @@
         <v>26</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C14" s="8" t="n">
         <v>0.55304</v>
@@ -7560,7 +7592,7 @@
         <v>31</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>13</v>
@@ -7600,7 +7632,7 @@
         <v>35</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>13</v>
@@ -7617,13 +7649,13 @@
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>9</v>
@@ -7660,10 +7692,10 @@
         <v>39</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>9</v>
@@ -7680,10 +7712,10 @@
         <v>39</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>9</v>
@@ -7763,7 +7795,7 @@
         <v>46</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>9</v>
@@ -7817,7 +7849,7 @@
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>7</v>
@@ -7837,7 +7869,7 @@
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>19</v>
@@ -7857,7 +7889,7 @@
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>48</v>
@@ -7920,10 +7952,10 @@
         <v>60</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>9</v>
@@ -7940,10 +7972,10 @@
         <v>60</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>9</v>
@@ -8023,7 +8055,7 @@
         <v>46</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>9</v>
@@ -8095,7 +8127,26 @@
         <v>-38.193144</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C43" s="8" t="n">
+        <v>0.442</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="E43" s="4" t="n">
+        <v>40.527483</v>
+      </c>
+      <c r="F43" s="5" t="n">
+        <v>-38.193144</v>
+      </c>
+    </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -9072,10 +9123,10 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
+      <selection pane="topLeft" activeCell="A36" activeCellId="1" sqref="A60:F60 A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.83"/>
@@ -9099,18 +9150,18 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C2" s="8" t="n">
         <v>0.56848</v>
@@ -9130,7 +9181,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C3" s="8" t="n">
         <v>0.20553</v>
@@ -9150,7 +9201,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C4" s="8" t="n">
         <v>0.382</v>
@@ -9170,7 +9221,7 @@
         <v>18</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C5" s="8" t="n">
         <v>0.20553</v>
@@ -9190,7 +9241,7 @@
         <v>18</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C6" s="8" t="n">
         <v>0.38896</v>
@@ -9250,7 +9301,7 @@
         <v>31</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C9" s="8" t="n">
         <v>0.20553</v>
@@ -9270,7 +9321,7 @@
         <v>25</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C10" s="8" t="n">
         <v>0.20553</v>
@@ -9370,7 +9421,7 @@
         <v>39</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C15" s="8" t="n">
         <v>0.0012</v>
@@ -9390,7 +9441,7 @@
         <v>39</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C16" s="8" t="n">
         <v>0.55304</v>
@@ -9527,7 +9578,7 @@
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>7</v>
@@ -9547,7 +9598,7 @@
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>19</v>
@@ -9567,7 +9618,7 @@
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>48</v>
@@ -9610,7 +9661,7 @@
         <v>60</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C27" s="8" t="n">
         <v>0.0012</v>
@@ -9630,7 +9681,7 @@
         <v>60</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C28" s="8" t="n">
         <v>0.55304</v>
@@ -9785,7 +9836,26 @@
         <v>-38.193144</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C36" s="8" t="n">
+        <v>0.442</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="E36" s="4" t="n">
+        <v>40.527483</v>
+      </c>
+      <c r="F36" s="5" t="n">
+        <v>-38.193144</v>
+      </c>
+    </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -10768,13 +10838,13 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B36" activeCellId="0" sqref="B36"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A141" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A174" activeCellId="1" sqref="A60:F60 A174"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="75.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="15" width="34.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.5"/>
@@ -10787,7 +10857,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="16" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -10810,19 +10880,19 @@
         <v>6</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C2" s="8" t="n">
         <v>0.514658864</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10830,19 +10900,19 @@
         <v>18</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C3" s="8" t="n">
         <v>0.514658864</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10850,19 +10920,19 @@
         <v>18</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C4" s="8" t="n">
         <v>0.514658864</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10870,19 +10940,19 @@
         <v>18</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C5" s="8" t="n">
         <v>0.514658864</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10890,19 +10960,19 @@
         <v>17</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C6" s="8" t="n">
         <v>0.514658864</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10930,19 +11000,19 @@
         <v>17</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C8" s="8" t="n">
         <v>0.514658864</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10950,19 +11020,19 @@
         <v>31</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C9" s="8" t="n">
         <v>0.514658864</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10970,19 +11040,19 @@
         <v>31</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C10" s="8" t="n">
         <v>0.514658864</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11050,19 +11120,19 @@
         <v>25</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C14" s="8" t="n">
         <v>0.514658864</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11070,19 +11140,19 @@
         <v>25</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C15" s="8" t="n">
         <v>0.514658864</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11130,7 +11200,7 @@
         <v>39</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C18" s="22" t="n">
         <v>0.2233</v>
@@ -11330,7 +11400,7 @@
         <v>39</v>
       </c>
       <c r="B28" s="21" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C28" s="22" t="n">
         <v>0.2233</v>
@@ -11570,7 +11640,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C40" s="22" t="n">
         <v>0.2233</v>
@@ -11670,7 +11740,7 @@
         <v>39</v>
       </c>
       <c r="B45" s="23" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C45" s="24" t="n">
         <v>0.2233</v>
@@ -11730,7 +11800,7 @@
         <v>39</v>
       </c>
       <c r="B48" s="21" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C48" s="22" t="n">
         <v>0.0617</v>
@@ -11750,7 +11820,7 @@
         <v>39</v>
       </c>
       <c r="B49" s="23" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C49" s="24" t="n">
         <v>0.0012</v>
@@ -11790,7 +11860,7 @@
         <v>39</v>
       </c>
       <c r="B51" s="23" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C51" s="24" t="n">
         <v>0.0012</v>
@@ -11850,7 +11920,7 @@
         <v>39</v>
       </c>
       <c r="B54" s="21" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C54" s="22" t="n">
         <v>0.0012</v>
@@ -11890,7 +11960,7 @@
         <v>39</v>
       </c>
       <c r="B56" s="21" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C56" s="22" t="n">
         <v>0.0012</v>
@@ -12030,13 +12100,13 @@
         <v>39</v>
       </c>
       <c r="B63" s="23" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C63" s="24" t="n">
         <v>0.516</v>
       </c>
       <c r="D63" s="23" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E63" s="6" t="n">
         <v>43.25</v>
@@ -12047,10 +12117,10 @@
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="18" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B64" s="21" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C64" s="22" t="n">
         <v>0.7341</v>
@@ -12070,7 +12140,7 @@
         <v>26</v>
       </c>
       <c r="B65" s="23" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C65" s="8" t="n">
         <v>0.377155625</v>
@@ -12090,7 +12160,7 @@
         <v>26</v>
       </c>
       <c r="B66" s="21" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C66" s="22" t="n">
         <v>0.42394</v>
@@ -12127,10 +12197,10 @@
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="18" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B68" s="21" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C68" s="22" t="n">
         <v>0.56848</v>
@@ -12147,10 +12217,10 @@
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="18" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B69" s="23" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C69" s="24" t="n">
         <v>0.56848</v>
@@ -12167,10 +12237,10 @@
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="18" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B70" s="21" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C70" s="22" t="n">
         <v>0.56848</v>
@@ -12187,7 +12257,7 @@
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="20" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B71" s="26" t="s">
         <v>19</v>
@@ -12201,15 +12271,15 @@
       <c r="E71" s="6" t="n">
         <v>45.516022</v>
       </c>
-      <c r="F71" s="27" t="n">
+      <c r="F71" s="7" t="n">
         <v>-122.681427</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="B72" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="B72" s="27" t="s">
         <v>19</v>
       </c>
       <c r="C72" s="22" t="n">
@@ -12227,9 +12297,9 @@
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="B73" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="B73" s="28" t="s">
         <v>19</v>
       </c>
       <c r="C73" s="24" t="n">
@@ -12241,13 +12311,13 @@
       <c r="E73" s="6" t="n">
         <v>45.516022</v>
       </c>
-      <c r="F73" s="27" t="n">
+      <c r="F73" s="7" t="n">
         <v>-122.681427</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="20" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B74" s="21" t="s">
         <v>7</v>
@@ -12267,7 +12337,7 @@
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="20" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B75" s="23" t="s">
         <v>48</v>
@@ -12287,7 +12357,7 @@
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="18" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B76" s="21" t="s">
         <v>59</v>
@@ -12307,7 +12377,7 @@
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="18" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B77" s="23" t="s">
         <v>59</v>
@@ -12327,7 +12397,7 @@
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="18" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B78" s="21" t="s">
         <v>59</v>
@@ -12347,7 +12417,7 @@
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="18" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B79" s="23" t="s">
         <v>59</v>
@@ -12367,10 +12437,10 @@
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="18" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B80" s="21" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C80" s="22" t="n">
         <v>0.58883</v>
@@ -12387,10 +12457,10 @@
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="18" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B81" s="23" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C81" s="24" t="n">
         <v>0.26818</v>
@@ -12407,7 +12477,7 @@
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="18" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B82" s="21" t="s">
         <v>53</v>
@@ -12427,7 +12497,7 @@
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="18" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B83" s="23" t="s">
         <v>27</v>
@@ -12447,10 +12517,10 @@
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="18" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B84" s="21" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C84" s="22" t="n">
         <v>0.700153846</v>
@@ -12467,16 +12537,16 @@
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="18" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B85" s="23" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C85" s="24" t="n">
         <v>0.516</v>
       </c>
       <c r="D85" s="23" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E85" s="6" t="n">
         <v>48.51667</v>
@@ -12581,7 +12651,7 @@
       <c r="E90" s="4" t="n">
         <v>39.907501</v>
       </c>
-      <c r="F90" s="30" t="n">
+      <c r="F90" s="5" t="n">
         <v>116.397232</v>
       </c>
     </row>
@@ -12590,7 +12660,7 @@
         <v>35</v>
       </c>
       <c r="B91" s="23" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C91" s="24" t="n">
         <v>0.982118481</v>
@@ -12606,7 +12676,7 @@
       </c>
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A92" s="31" t="s">
+      <c r="A92" s="29" t="s">
         <v>58</v>
       </c>
       <c r="B92" s="21" t="s">
@@ -12626,7 +12696,7 @@
       </c>
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A93" s="31" t="s">
+      <c r="A93" s="29" t="s">
         <v>58</v>
       </c>
       <c r="B93" s="23" t="s">
@@ -12646,7 +12716,7 @@
       </c>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A94" s="31" t="s">
+      <c r="A94" s="29" t="s">
         <v>58</v>
       </c>
       <c r="B94" s="21" t="s">
@@ -12666,7 +12736,7 @@
       </c>
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A95" s="31" t="s">
+      <c r="A95" s="29" t="s">
         <v>58</v>
       </c>
       <c r="B95" s="23" t="s">
@@ -12686,7 +12756,7 @@
       </c>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A96" s="31" t="s">
+      <c r="A96" s="29" t="s">
         <v>58</v>
       </c>
       <c r="B96" s="21" t="s">
@@ -12706,7 +12776,7 @@
       </c>
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A97" s="31" t="s">
+      <c r="A97" s="29" t="s">
         <v>58</v>
       </c>
       <c r="B97" s="23" t="s">
@@ -12726,7 +12796,7 @@
       </c>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A98" s="31" t="s">
+      <c r="A98" s="29" t="s">
         <v>58</v>
       </c>
       <c r="B98" s="21" t="s">
@@ -12746,7 +12816,7 @@
       </c>
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A99" s="31" t="s">
+      <c r="A99" s="29" t="s">
         <v>58</v>
       </c>
       <c r="B99" s="23" t="s">
@@ -12766,7 +12836,7 @@
       </c>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A100" s="31" t="s">
+      <c r="A100" s="29" t="s">
         <v>58</v>
       </c>
       <c r="B100" s="21" t="s">
@@ -12786,7 +12856,7 @@
       </c>
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A101" s="32" t="s">
+      <c r="A101" s="30" t="s">
         <v>33</v>
       </c>
       <c r="B101" s="23" t="s">
@@ -12806,11 +12876,11 @@
       </c>
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A102" s="32" t="s">
+      <c r="A102" s="30" t="s">
         <v>33</v>
       </c>
       <c r="B102" s="21" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C102" s="22" t="n">
         <v>0.2524</v>
@@ -12826,11 +12896,11 @@
       </c>
     </row>
     <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A103" s="32" t="s">
+      <c r="A103" s="30" t="s">
         <v>33</v>
       </c>
       <c r="B103" s="23" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C103" s="24" t="n">
         <v>0.38896</v>
@@ -12846,11 +12916,11 @@
       </c>
     </row>
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A104" s="32" t="s">
+      <c r="A104" s="30" t="s">
         <v>33</v>
       </c>
       <c r="B104" s="21" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C104" s="22" t="n">
         <v>0.38896</v>
@@ -12866,11 +12936,11 @@
       </c>
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A105" s="32" t="s">
+      <c r="A105" s="30" t="s">
         <v>33</v>
       </c>
       <c r="B105" s="23" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C105" s="24" t="n">
         <v>0.36338</v>
@@ -12886,11 +12956,11 @@
       </c>
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A106" s="32" t="s">
+      <c r="A106" s="30" t="s">
         <v>33</v>
       </c>
       <c r="B106" s="21" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C106" s="22" t="n">
         <v>0.20553</v>
@@ -12906,11 +12976,11 @@
       </c>
     </row>
     <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A107" s="32" t="s">
+      <c r="A107" s="30" t="s">
         <v>33</v>
       </c>
       <c r="B107" s="23" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C107" s="24" t="n">
         <v>0.2524</v>
@@ -12926,11 +12996,11 @@
       </c>
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A108" s="32" t="s">
+      <c r="A108" s="30" t="s">
         <v>33</v>
       </c>
       <c r="B108" s="21" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C108" s="22" t="n">
         <v>0.20553</v>
@@ -12946,7 +13016,7 @@
       </c>
     </row>
     <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A109" s="32" t="s">
+      <c r="A109" s="30" t="s">
         <v>33</v>
       </c>
       <c r="B109" s="23" t="s">
@@ -12966,7 +13036,7 @@
       </c>
     </row>
     <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A110" s="32" t="s">
+      <c r="A110" s="30" t="s">
         <v>33</v>
       </c>
       <c r="B110" s="21" t="s">
@@ -12986,11 +13056,11 @@
       </c>
     </row>
     <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A111" s="32" t="s">
+      <c r="A111" s="30" t="s">
         <v>33</v>
       </c>
       <c r="B111" s="23" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C111" s="24" t="n">
         <v>0.20553</v>
@@ -13006,11 +13076,11 @@
       </c>
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A112" s="32" t="s">
+      <c r="A112" s="30" t="s">
         <v>33</v>
       </c>
       <c r="B112" s="21" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C112" s="22" t="n">
         <v>0.20553</v>
@@ -13026,11 +13096,11 @@
       </c>
     </row>
     <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A113" s="32" t="s">
+      <c r="A113" s="30" t="s">
         <v>33</v>
       </c>
       <c r="B113" s="23" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C113" s="24" t="n">
         <v>0.38896</v>
@@ -13046,7 +13116,7 @@
       </c>
     </row>
     <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A114" s="32" t="s">
+      <c r="A114" s="30" t="s">
         <v>33</v>
       </c>
       <c r="B114" s="21" t="s">
@@ -13058,7 +13128,7 @@
       <c r="D114" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="E114" s="33" t="n">
+      <c r="E114" s="4" t="n">
         <v>39.907501</v>
       </c>
       <c r="F114" s="5" t="n">
@@ -13066,11 +13136,11 @@
       </c>
     </row>
     <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A115" s="32" t="s">
+      <c r="A115" s="30" t="s">
         <v>33</v>
       </c>
       <c r="B115" s="23" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C115" s="24" t="n">
         <v>0.20553</v>
@@ -13086,11 +13156,11 @@
       </c>
     </row>
     <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A116" s="32" t="s">
+      <c r="A116" s="30" t="s">
         <v>33</v>
       </c>
       <c r="B116" s="21" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C116" s="22" t="n">
         <v>0.01152</v>
@@ -13106,7 +13176,7 @@
       </c>
     </row>
     <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A117" s="32" t="s">
+      <c r="A117" s="30" t="s">
         <v>33</v>
       </c>
       <c r="B117" s="23" t="s">
@@ -13126,7 +13196,7 @@
       </c>
     </row>
     <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A118" s="32" t="s">
+      <c r="A118" s="30" t="s">
         <v>33</v>
       </c>
       <c r="B118" s="21" t="s">
@@ -13146,11 +13216,11 @@
       </c>
     </row>
     <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A119" s="34" t="s">
+      <c r="A119" s="30" t="s">
         <v>33</v>
       </c>
       <c r="B119" s="23" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C119" s="24" t="n">
         <v>0.20553</v>
@@ -13166,11 +13236,11 @@
       </c>
     </row>
     <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A120" s="32" t="s">
+      <c r="A120" s="30" t="s">
         <v>33</v>
       </c>
       <c r="B120" s="21" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C120" s="22" t="n">
         <v>0.38896</v>
@@ -13186,11 +13256,11 @@
       </c>
     </row>
     <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A121" s="32" t="s">
+      <c r="A121" s="30" t="s">
         <v>33</v>
       </c>
       <c r="B121" s="23" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C121" s="24" t="n">
         <v>0.71022</v>
@@ -13206,7 +13276,7 @@
       </c>
     </row>
     <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A122" s="32" t="s">
+      <c r="A122" s="30" t="s">
         <v>33</v>
       </c>
       <c r="B122" s="21" t="s">
@@ -13226,11 +13296,11 @@
       </c>
     </row>
     <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A123" s="32" t="s">
+      <c r="A123" s="30" t="s">
         <v>33</v>
       </c>
       <c r="B123" s="23" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C123" s="24" t="n">
         <v>0.71022</v>
@@ -13246,7 +13316,7 @@
       </c>
     </row>
     <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A124" s="31" t="s">
+      <c r="A124" s="29" t="s">
         <v>56</v>
       </c>
       <c r="B124" s="21" t="s">
@@ -13310,7 +13380,7 @@
         <v>60</v>
       </c>
       <c r="B127" s="21" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C127" s="22" t="n">
         <v>0.2233</v>
@@ -13510,7 +13580,7 @@
         <v>60</v>
       </c>
       <c r="B137" s="21" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C137" s="22" t="n">
         <v>0.2233</v>
@@ -13750,7 +13820,7 @@
         <v>60</v>
       </c>
       <c r="B149" s="21" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C149" s="22" t="n">
         <v>0.2233</v>
@@ -13850,7 +13920,7 @@
         <v>60</v>
       </c>
       <c r="B154" s="23" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C154" s="24" t="n">
         <v>0.2233</v>
@@ -13910,7 +13980,7 @@
         <v>60</v>
       </c>
       <c r="B157" s="21" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C157" s="22" t="n">
         <v>0.0617</v>
@@ -13930,7 +14000,7 @@
         <v>60</v>
       </c>
       <c r="B158" s="23" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C158" s="24" t="n">
         <v>0.0012</v>
@@ -13970,7 +14040,7 @@
         <v>60</v>
       </c>
       <c r="B160" s="23" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C160" s="24" t="n">
         <v>0.0012</v>
@@ -14030,7 +14100,7 @@
         <v>60</v>
       </c>
       <c r="B163" s="21" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C163" s="22" t="n">
         <v>0.0012</v>
@@ -14070,7 +14140,7 @@
         <v>60</v>
       </c>
       <c r="B165" s="21" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C165" s="22" t="n">
         <v>0.0012</v>
@@ -14210,13 +14280,13 @@
         <v>60</v>
       </c>
       <c r="B172" s="23" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C172" s="24" t="n">
         <v>0.516</v>
       </c>
       <c r="D172" s="23" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E172" s="6" t="n">
         <v>43.25</v>
@@ -14245,7 +14315,26 @@
         <v>-38.193144</v>
       </c>
     </row>
-    <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A174" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B174" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C174" s="8" t="n">
+        <v>0.442</v>
+      </c>
+      <c r="D174" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="E174" s="4" t="n">
+        <v>40.527483</v>
+      </c>
+      <c r="F174" s="5" t="n">
+        <v>-38.193144</v>
+      </c>
+    </row>
     <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="176" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>